<commit_message>
Add Workbook.set() method to allow workbook to be generated from JSON data
</commit_message>
<xml_diff>
--- a/test/files/print.xlsx
+++ b/test/files/print.xlsx
@@ -63851,21 +63851,21 @@
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" scale="50"/>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="90" man="1"/>
-    <brk id="180" man="1"/>
-    <brk id="270" man="1"/>
+    <brk id="90" man="1" max="1048575"/>
+    <brk id="180" man="1" max="1048575"/>
+    <brk id="270" man="1" max="1048575"/>
   </rowBreaks>
   <colBreaks count="10" manualBreakCount="10">
-    <brk id="15" man="1"/>
-    <brk id="30" man="1"/>
-    <brk id="45" man="1"/>
-    <brk id="60" man="1"/>
-    <brk id="75" man="1"/>
-    <brk id="90" man="1"/>
-    <brk id="105" man="1"/>
-    <brk id="120" man="1"/>
-    <brk id="135" man="1"/>
-    <brk id="150" man="1"/>
+    <brk id="15" man="1" max="1048575"/>
+    <brk id="30" man="1" max="1048575"/>
+    <brk id="45" man="1" max="1048575"/>
+    <brk id="60" man="1" max="1048575"/>
+    <brk id="75" man="1" max="1048575"/>
+    <brk id="90" man="1" max="1048575"/>
+    <brk id="105" man="1" max="1048575"/>
+    <brk id="120" man="1" max="1048575"/>
+    <brk id="135" man="1" max="1048575"/>
+    <brk id="150" man="1" max="1048575"/>
   </colBreaks>
 </worksheet>
 </file>
</xml_diff>